<commit_message>
Add email field to User model
</commit_message>
<xml_diff>
--- a/Sample Data/sample_dataset - CMUPoll.xlsx
+++ b/Sample Data/sample_dataset - CMUPoll.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sung/Documents/67442/CMUPoll/Sample Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sung/Documents/67442/cmu_polls/Sample Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F2CC28-7CB8-4948-82ED-7498D8555089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809E0134-4C2A-F742-A5C1-D889824F02DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1600" windowWidth="33600" windowHeight="17140" activeTab="8" xr2:uid="{7DB1CFF2-D673-4A4A-84BB-12361BFD39C9}"/>
+    <workbookView xWindow="0" yWindow="1600" windowWidth="33600" windowHeight="17140" xr2:uid="{7DB1CFF2-D673-4A4A-84BB-12361BFD39C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="136">
   <si>
     <t>id</t>
   </si>
@@ -426,6 +426,27 @@
   </si>
   <si>
     <t>tag_id</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>yonghool@andrew.cmu.edu</t>
+  </si>
+  <si>
+    <t>siheonl@andrew.cmu.edu</t>
+  </si>
+  <si>
+    <t>sunghoch@andrew.cmu.edu</t>
+  </si>
+  <si>
+    <t>xinrany@andrew.cmu.edu</t>
+  </si>
+  <si>
+    <t>profh@cmu.edu</t>
+  </si>
+  <si>
+    <t>andykim@andrew.cmu.edu</t>
   </si>
 </sst>
 </file>
@@ -825,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3B10964-3AA5-814C-8358-AF2FC19C67C1}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,7 +857,7 @@
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -847,16 +868,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -866,17 +890,20 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1230</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -886,17 +913,20 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4124</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -906,17 +936,20 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1231</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -926,17 +959,20 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>214</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -946,17 +982,20 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4124</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -966,17 +1005,28 @@
       <c r="C7" t="s">
         <v>65</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" t="s">
         <v>69</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2024</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{864FF845-FB92-1744-A3C2-A615CF5FBDE3}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{1A068532-3C4B-C14F-B397-D9CD94EBE6ED}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{7370648E-D4E9-CA46-A422-1A52C5A7EAF9}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{BD62FD5C-A58C-704E-ACC8-50CD1370E2DE}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{7B6B0C6D-3A37-3242-A54B-1FC3E4CDB620}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{05725700-E3A5-184B-AB22-A5932CC5FD73}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3007,7 +3057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABC80E2-7B95-BC44-8892-4388E3488EC4}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+    <sheetView zoomScale="158" workbookViewId="0">
       <selection sqref="A1:B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Enable answering polls funtionality
</commit_message>
<xml_diff>
--- a/Sample Data/sample_dataset - CMUPoll.xlsx
+++ b/Sample Data/sample_dataset - CMUPoll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sung/Documents/67442/cmu_polls/Sample Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1378B498-0FDF-0B41-BF29-5000B75A03F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9EB8B7-63C9-C647-B9FB-5195FB8ECB91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40240" yWindow="2720" windowWidth="33600" windowHeight="17140" xr2:uid="{7DB1CFF2-D673-4A4A-84BB-12361BFD39C9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19700" activeTab="6" xr2:uid="{7DB1CFF2-D673-4A4A-84BB-12361BFD39C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3B10964-3AA5-814C-8358-AF2FC19C67C1}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,6 +1028,7 @@
     <hyperlink ref="D7" r:id="rId6" xr:uid="{05725700-E3A5-184B-AB22-A5932CC5FD73}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1523,7 +1524,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScale="142" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1842,7 +1843,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="D12" sqref="A1:D12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2066,7 +2067,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScale="144" workbookViewId="0">
-      <selection sqref="A1:C31"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2455,8 +2456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0D61FB-7176-D747-8C34-75D863962137}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2504,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2532,7 +2533,7 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -2549,7 +2550,7 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2566,7 +2567,7 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -2583,7 +2584,7 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -2600,7 +2601,7 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -2617,7 +2618,7 @@
         <v>6</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -2634,7 +2635,7 @@
         <v>7</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2651,7 +2652,7 @@
         <v>8</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2668,7 +2669,7 @@
         <v>3</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -2685,7 +2686,7 @@
         <v>9</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -2702,7 +2703,7 @@
         <v>10</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2716,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2730,7 +2731,7 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2744,7 +2745,7 @@
         <v>7</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2758,7 +2759,7 @@
         <v>10</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2786,7 +2787,7 @@
         <v>8</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update sample tag data and update 'create' function in Tag model
</commit_message>
<xml_diff>
--- a/Sample Data/sample_dataset - CMUPoll.xlsx
+++ b/Sample Data/sample_dataset - CMUPoll.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sung/Documents/67442/cmu_polls/Sample Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9EB8B7-63C9-C647-B9FB-5195FB8ECB91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA4B9A-21C6-7F48-81EA-5AF60B0E278E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19700" activeTab="6" xr2:uid="{7DB1CFF2-D673-4A4A-84BB-12361BFD39C9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19100" activeTab="7" xr2:uid="{7DB1CFF2-D673-4A4A-84BB-12361BFD39C9}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="134">
   <si>
     <t>id</t>
   </si>
@@ -279,12 +279,6 @@
   </si>
   <si>
     <t>www.cmupoll.com/poll9</t>
-  </si>
-  <si>
-    <t>"life"</t>
-  </si>
-  <si>
-    <t>"place"</t>
   </si>
   <si>
     <t>"Information Systems"</t>
@@ -868,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -891,7 +885,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -914,7 +908,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -931,13 +925,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -960,7 +954,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -983,7 +977,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
@@ -1006,7 +1000,7 @@
         <v>65</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
         <v>69</v>
@@ -1892,7 +1886,7 @@
         <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2022,7 +2016,7 @@
         <v>40</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2039,7 +2033,7 @@
         <v>40</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2081,10 +2075,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2095,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2106,7 +2100,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2117,7 +2111,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2128,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -2142,7 +2136,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2156,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -2170,7 +2164,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -2184,7 +2178,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -2198,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -2212,7 +2206,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2226,7 +2220,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2240,7 +2234,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -2254,7 +2248,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -2268,7 +2262,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2279,7 +2273,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2290,7 +2284,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2301,7 +2295,7 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2312,7 +2306,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2323,7 +2317,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2334,7 +2328,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2345,7 +2339,7 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2356,7 +2350,7 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2367,7 +2361,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2378,7 +2372,7 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2389,7 +2383,7 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2400,7 +2394,7 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2411,7 +2405,7 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2422,7 +2416,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2433,7 +2427,7 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2444,7 +2438,7 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2456,7 +2450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0D61FB-7176-D747-8C34-75D863962137}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+    <sheetView zoomScale="144" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -2474,10 +2468,10 @@
         <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2799,8 +2793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD82C4DF-F26B-5841-9034-38722ADD6015}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="158" workbookViewId="0">
-      <selection sqref="A1:C21"/>
+    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
+      <selection activeCell="C21" sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2816,7 +2810,7 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2895,7 +2889,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -2907,7 +2901,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -2919,7 +2913,7 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -2931,7 +2925,7 @@
         <v>4</v>
       </c>
       <c r="C11">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -2943,7 +2937,7 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -2955,7 +2949,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -2967,7 +2961,7 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F14" s="4"/>
     </row>
@@ -2979,7 +2973,7 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F15" s="5"/>
     </row>
@@ -2991,7 +2985,7 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3002,7 +2996,7 @@
         <v>8</v>
       </c>
       <c r="C17">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3013,7 +3007,7 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3024,7 +3018,7 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3035,7 +3029,7 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -3046,7 +3040,7 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3056,10 +3050,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABC80E2-7B95-BC44-8892-4388E3488EC4}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView zoomScale="158" workbookViewId="0">
-      <selection sqref="A1:B21"/>
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3080,7 +3074,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3088,7 +3082,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3096,7 +3090,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3112,7 +3106,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -3121,7 +3115,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -3130,7 +3124,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -3139,7 +3133,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -3148,7 +3142,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -3157,7 +3151,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -3175,7 +3169,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -3184,7 +3178,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" s="4"/>
     </row>
@@ -3196,54 +3190,6 @@
         <v>88</v>
       </c>
       <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>90</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>